<commit_message>
SIMCC BD CSV - Ajustes
</commit_message>
<xml_diff>
--- a/Files/researcher_ufsb.xlsx
+++ b/Files/researcher_ufsb.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Arch\home\lilith\repository\back_simcc\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Arch\home\lilith\repository\back_end_simcc\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3884BBE7-EC2B-43D5-A575-CB1151CC56F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DA224D-8DD2-48EE-A0EB-E8C3DC464539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11295" xr2:uid="{A80C27C4-474D-854B-B118-BB800353428A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A80C27C4-474D-854B-B118-BB800353428A}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -2023,7 +2023,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00,000,000,0\-00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2043,8 +2043,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2055,6 +2062,11 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -2078,10 +2090,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2101,8 +2114,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bom" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
@@ -2516,16 +2531,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED26D68-EB40-464D-9E56-6902448E8394}">
-  <dimension ref="A1:B333"/>
+  <dimension ref="A1:D333"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44" customWidth="1"/>
     <col min="2" max="2" width="21.375" customWidth="1"/>
+    <col min="3" max="3" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -4064,7 +4080,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
         <v>380</v>
       </c>
@@ -4072,7 +4088,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>382</v>
       </c>
@@ -4080,7 +4096,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
         <v>384</v>
       </c>
@@ -4088,7 +4104,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>386</v>
       </c>
@@ -4096,7 +4112,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
         <v>388</v>
       </c>
@@ -4104,7 +4120,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>390</v>
       </c>
@@ -4112,7 +4128,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
         <v>392</v>
       </c>
@@ -4120,7 +4136,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>394</v>
       </c>
@@ -4128,15 +4144,17 @@
         <v>395</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
         <v>396</v>
       </c>
       <c r="B201" s="4" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C201" s="7"/>
+      <c r="D201" s="7"/>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>398</v>
       </c>
@@ -4144,7 +4162,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
         <v>400</v>
       </c>
@@ -4152,7 +4170,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>402</v>
       </c>
@@ -4160,7 +4178,7 @@
         <v>94505063534</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
         <v>403</v>
       </c>
@@ -4168,7 +4186,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>405</v>
       </c>
@@ -4176,7 +4194,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
         <v>407</v>
       </c>
@@ -4184,7 +4202,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>409</v>
       </c>
@@ -5220,6 +5238,6 @@
     <cfRule type="duplicateValues" dxfId="0" priority="11" stopIfTrue="1"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>